<commit_message>
Finallized pin arrangements and updated SteallarisPort to use new pin assignments.
</commit_message>
<xml_diff>
--- a/docs/GRP_Proto_Pins.xlsx
+++ b/docs/GRP_Proto_Pins.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="480" yWindow="75" windowWidth="18195" windowHeight="11820"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="135">
   <si>
     <t>GND</t>
   </si>
@@ -415,13 +415,19 @@
   </si>
   <si>
     <t>PA2</t>
+  </si>
+  <si>
+    <t>Actuators</t>
+  </si>
+  <si>
+    <t>Sensors</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -451,7 +457,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -506,6 +512,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="4">
     <border>
@@ -552,7 +564,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -654,21 +666,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -711,10 +727,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -734,7 +750,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -766,10 +782,10 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -789,7 +805,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -878,7 +894,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -913,7 +928,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1089,23 +1103,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="C4:AF72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T52" sqref="T52"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T46" sqref="T46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="30" width="5.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:27">
       <c r="C4" s="3">
         <v>1</v>
       </c>
@@ -1182,7 +1196,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:27">
       <c r="C5" s="12" t="s">
         <v>0</v>
       </c>
@@ -1261,7 +1275,7 @@
         <v>+5v</v>
       </c>
     </row>
-    <row r="6" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:27">
       <c r="C6" s="12" t="s">
         <v>0</v>
       </c>
@@ -1340,7 +1354,7 @@
         <v>+5V</v>
       </c>
     </row>
-    <row r="7" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:27">
       <c r="C7" s="1">
         <v>2</v>
       </c>
@@ -1417,29 +1431,29 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="3:27" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="D9" s="36" t="s">
+    <row r="9" spans="3:27" ht="23.25">
+      <c r="D9" s="44" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
-      <c r="G9" s="36"/>
-      <c r="H9" s="36"/>
-      <c r="I9" s="36"/>
-      <c r="J9" s="36"/>
-      <c r="K9" s="36"/>
-      <c r="L9" s="36"/>
-      <c r="M9" s="36"/>
-      <c r="N9" s="36"/>
-      <c r="O9" s="36"/>
-      <c r="P9" s="36"/>
-      <c r="Q9" s="36"/>
-      <c r="R9" s="36"/>
-      <c r="S9" s="36"/>
-      <c r="T9" s="36"/>
-      <c r="U9" s="36"/>
-    </row>
-    <row r="10" spans="3:27" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="E9" s="44"/>
+      <c r="F9" s="44"/>
+      <c r="G9" s="44"/>
+      <c r="H9" s="44"/>
+      <c r="I9" s="44"/>
+      <c r="J9" s="44"/>
+      <c r="K9" s="44"/>
+      <c r="L9" s="44"/>
+      <c r="M9" s="44"/>
+      <c r="N9" s="44"/>
+      <c r="O9" s="44"/>
+      <c r="P9" s="44"/>
+      <c r="Q9" s="44"/>
+      <c r="R9" s="44"/>
+      <c r="S9" s="44"/>
+      <c r="T9" s="44"/>
+      <c r="U9" s="44"/>
+    </row>
+    <row r="10" spans="3:27" ht="23.25">
       <c r="D10" s="11"/>
       <c r="E10" s="11"/>
       <c r="F10" s="11"/>
@@ -1459,7 +1473,7 @@
       <c r="T10" s="11"/>
       <c r="U10" s="11"/>
     </row>
-    <row r="11" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:27">
       <c r="D11" s="10"/>
       <c r="E11" s="10"/>
       <c r="F11" s="10"/>
@@ -1479,7 +1493,7 @@
       <c r="T11" s="10"/>
       <c r="U11" s="10"/>
     </row>
-    <row r="12" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:27">
       <c r="D12" s="10"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
@@ -1499,7 +1513,7 @@
       <c r="T12" s="10"/>
       <c r="U12" s="10"/>
     </row>
-    <row r="13" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:27">
       <c r="D13" s="10"/>
       <c r="E13" s="10"/>
       <c r="F13" s="10"/>
@@ -1519,7 +1533,7 @@
       <c r="T13" s="10"/>
       <c r="U13" s="10"/>
     </row>
-    <row r="14" spans="3:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:27" ht="15" customHeight="1">
       <c r="D14" s="10"/>
       <c r="E14" s="10"/>
       <c r="F14" s="10"/>
@@ -1539,31 +1553,31 @@
       <c r="T14" s="10"/>
       <c r="U14" s="10"/>
     </row>
-    <row r="15" spans="3:27" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:27" ht="15" customHeight="1">
       <c r="D15" s="10"/>
-      <c r="E15" s="35" t="s">
+      <c r="E15" s="42" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="35"/>
-      <c r="G15" s="35"/>
-      <c r="H15" s="35"/>
-      <c r="I15" s="35"/>
-      <c r="J15" s="35"/>
+      <c r="F15" s="42"/>
+      <c r="G15" s="42"/>
+      <c r="H15" s="42"/>
+      <c r="I15" s="42"/>
+      <c r="J15" s="42"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
-      <c r="O15" s="35" t="s">
+      <c r="O15" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="P15" s="35"/>
-      <c r="Q15" s="35"/>
-      <c r="R15" s="35"/>
-      <c r="S15" s="35"/>
-      <c r="T15" s="35"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="42"/>
+      <c r="R15" s="42"/>
+      <c r="S15" s="42"/>
+      <c r="T15" s="42"/>
       <c r="U15" s="10"/>
     </row>
-    <row r="16" spans="3:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:27">
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
@@ -1585,7 +1599,7 @@
       <c r="U16" s="10"/>
       <c r="V16" s="10"/>
     </row>
-    <row r="18" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:32">
       <c r="C18" s="16">
         <v>13</v>
       </c>
@@ -1665,7 +1679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:32">
       <c r="C19" s="28" t="str">
         <f t="shared" ref="C19:N19" si="0">LOOKUP(C18,$C$25:$C$49,$E$25:$E$49)</f>
         <v>C2-2</v>
@@ -1771,7 +1785,7 @@
         <v>C2-3</v>
       </c>
     </row>
-    <row r="20" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:32">
       <c r="C20" s="15"/>
       <c r="D20" s="29" t="str">
         <f t="shared" ref="D20:N20" si="2">LOOKUP(D21,$C$25:$C$49,$E$25:$E$49)</f>
@@ -1871,7 +1885,7 @@
         <v>C2-4</v>
       </c>
     </row>
-    <row r="21" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:32">
       <c r="D21" s="17">
         <v>25</v>
       </c>
@@ -1945,32 +1959,32 @@
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="3:32">
       <c r="D22" s="15"/>
       <c r="E22" s="15"/>
-      <c r="F22" s="34" t="s">
+      <c r="F22" s="43" t="s">
         <v>41</v>
       </c>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+      <c r="K22" s="43"/>
+      <c r="L22" s="43"/>
       <c r="M22" s="15"/>
       <c r="N22" s="15"/>
       <c r="O22" s="15"/>
-      <c r="T22" s="34" t="s">
+      <c r="T22" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="U22" s="34"/>
-      <c r="V22" s="34"/>
-      <c r="W22" s="34"/>
-      <c r="X22" s="34"/>
-      <c r="Y22" s="34"/>
-      <c r="Z22" s="34"/>
-    </row>
-    <row r="23" spans="3:32" x14ac:dyDescent="0.25">
+      <c r="U22" s="43"/>
+      <c r="V22" s="43"/>
+      <c r="W22" s="43"/>
+      <c r="X22" s="43"/>
+      <c r="Y22" s="43"/>
+      <c r="Z22" s="43"/>
+    </row>
+    <row r="23" spans="3:32">
       <c r="D23" s="15"/>
       <c r="E23" s="15"/>
       <c r="F23" s="15"/>
@@ -1990,7 +2004,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="3:32">
       <c r="C24" s="2" t="s">
         <v>37</v>
       </c>
@@ -2017,7 +2031,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:32">
       <c r="C25" s="2">
         <v>1</v>
       </c>
@@ -2046,7 +2060,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="26" spans="3:32">
       <c r="C26" s="2">
         <v>2</v>
       </c>
@@ -2077,7 +2091,7 @@
       <c r="W26" s="10" t="s">
         <v>117</v>
       </c>
-      <c r="X26" s="40" t="s">
+      <c r="X26" s="37" t="s">
         <v>14</v>
       </c>
       <c r="Z26" t="s">
@@ -2094,7 +2108,7 @@
         <v>C0-7</v>
       </c>
     </row>
-    <row r="27" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="27" spans="3:32">
       <c r="C27" s="2">
         <v>3</v>
       </c>
@@ -2125,13 +2139,13 @@
       <c r="W27" s="10" t="s">
         <v>118</v>
       </c>
-      <c r="X27" s="40" t="s">
+      <c r="X27" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="Y27" s="37" t="s">
+      <c r="Y27" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="Z27" s="42" t="s">
+      <c r="Z27" s="39" t="s">
         <v>127</v>
       </c>
       <c r="AC27" t="s">
@@ -2141,7 +2155,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="28" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:32">
       <c r="C28" s="2">
         <v>4</v>
       </c>
@@ -2166,19 +2180,19 @@
       <c r="P28" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="Q28" s="40" t="s">
+      <c r="Q28" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="R28" s="37" t="s">
+      <c r="R28" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="S28" s="42" t="s">
+      <c r="S28" s="39" t="s">
         <v>107</v>
       </c>
       <c r="W28" s="10" t="s">
         <v>119</v>
       </c>
-      <c r="X28" s="40" t="s">
+      <c r="X28" s="37" t="s">
         <v>18</v>
       </c>
       <c r="AC28" t="s">
@@ -2188,7 +2202,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:32">
       <c r="C29" s="2">
         <v>5</v>
       </c>
@@ -2213,19 +2227,19 @@
       <c r="P29" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="Q29" s="40" t="s">
+      <c r="Q29" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="R29" s="37" t="s">
+      <c r="R29" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="S29" s="42" t="s">
+      <c r="S29" s="39" t="s">
         <v>108</v>
       </c>
       <c r="W29" s="10" t="s">
         <v>120</v>
       </c>
-      <c r="X29" s="40" t="s">
+      <c r="X29" s="37" t="s">
         <v>20</v>
       </c>
       <c r="AC29" t="s">
@@ -2235,7 +2249,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="30" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:32">
       <c r="C30" s="2">
         <v>6</v>
       </c>
@@ -2260,19 +2274,19 @@
       <c r="P30" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="Q30" s="40" t="s">
+      <c r="Q30" s="37" t="s">
         <v>19</v>
       </c>
-      <c r="R30" s="37" t="s">
+      <c r="R30" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="S30" s="42" t="s">
+      <c r="S30" s="39" t="s">
         <v>109</v>
       </c>
       <c r="W30" s="10" t="s">
         <v>121</v>
       </c>
-      <c r="X30" s="41" t="s">
+      <c r="X30" s="38" t="s">
         <v>33</v>
       </c>
       <c r="AC30" t="s">
@@ -2282,7 +2296,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:32">
       <c r="C31" s="2">
         <v>7</v>
       </c>
@@ -2307,25 +2321,25 @@
       <c r="P31" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="Q31" s="40" t="s">
+      <c r="Q31" s="37" t="s">
         <v>17</v>
       </c>
-      <c r="R31" s="37" t="s">
+      <c r="R31" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="S31" s="42" t="s">
+      <c r="S31" s="39" t="s">
         <v>110</v>
       </c>
       <c r="W31" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="X31" s="41" t="s">
+      <c r="X31" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="Y31" s="37" t="s">
+      <c r="Y31" s="35" t="s">
         <v>7</v>
       </c>
-      <c r="Z31" s="42" t="s">
+      <c r="Z31" s="39" t="s">
         <v>128</v>
       </c>
       <c r="AC31" t="s">
@@ -2335,7 +2349,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="32" spans="3:32" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:32">
       <c r="C32" s="2">
         <v>8</v>
       </c>
@@ -2360,25 +2374,25 @@
       <c r="P32" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="Q32" s="41" t="s">
+      <c r="Q32" s="38" t="s">
         <v>30</v>
       </c>
-      <c r="R32" s="38" t="s">
+      <c r="R32" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="S32" s="42" t="s">
+      <c r="S32" s="39" t="s">
         <v>111</v>
       </c>
       <c r="W32" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="X32" s="41" t="s">
+      <c r="X32" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="Y32" s="37" t="s">
+      <c r="Y32" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="Z32" s="42" t="s">
+      <c r="Z32" s="39" t="s">
         <v>129</v>
       </c>
       <c r="AC32" t="s">
@@ -2388,7 +2402,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="33" spans="3:30">
       <c r="C33" s="2">
         <v>9</v>
       </c>
@@ -2413,25 +2427,25 @@
       <c r="P33" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="Q33" s="41" t="s">
+      <c r="Q33" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="R33" s="38" t="s">
+      <c r="R33" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="S33" s="42" t="s">
+      <c r="S33" s="39" t="s">
         <v>112</v>
       </c>
       <c r="W33" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="X33" s="41" t="s">
+      <c r="X33" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="Y33" s="37" t="s">
+      <c r="Y33" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="Z33" s="42" t="s">
+      <c r="Z33" s="39" t="s">
         <v>130</v>
       </c>
       <c r="AC33" t="s">
@@ -2441,7 +2455,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="34" spans="3:30">
       <c r="C34" s="2">
         <v>10</v>
       </c>
@@ -2466,25 +2480,25 @@
       <c r="P34" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="Q34" s="41" t="s">
+      <c r="Q34" s="38" t="s">
         <v>32</v>
       </c>
-      <c r="R34" s="38" t="s">
+      <c r="R34" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="S34" s="42" t="s">
+      <c r="S34" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="W34" s="42" t="s">
+      <c r="W34" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="X34" s="43" t="s">
+      <c r="X34" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="Y34" s="38" t="s">
+      <c r="Y34" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="Z34" s="42" t="s">
+      <c r="Z34" s="39" t="s">
         <v>131</v>
       </c>
       <c r="AC34" t="s">
@@ -2494,7 +2508,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="35" spans="3:30">
       <c r="C35" s="2">
         <v>11</v>
       </c>
@@ -2519,25 +2533,25 @@
       <c r="P35" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="Q35" s="41" t="s">
+      <c r="Q35" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="R35" s="38" t="s">
+      <c r="R35" s="36" t="s">
         <v>27</v>
       </c>
-      <c r="S35" s="42" t="s">
+      <c r="S35" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="W35" s="42" t="s">
+      <c r="W35" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="X35" s="43" t="s">
+      <c r="X35" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="Y35" s="38" t="s">
+      <c r="Y35" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="Z35" s="42" t="s">
+      <c r="Z35" s="39" t="s">
         <v>132</v>
       </c>
       <c r="AC35" t="s">
@@ -2547,7 +2561,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="36" spans="3:30">
       <c r="C36" s="2">
         <v>12</v>
       </c>
@@ -2576,7 +2590,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="37" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="37" spans="3:30">
       <c r="C37" s="2">
         <v>13</v>
       </c>
@@ -2598,14 +2612,14 @@
         <f t="shared" si="5"/>
         <v>+5V</v>
       </c>
-      <c r="P37" s="35" t="s">
+      <c r="P37" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="Q37" s="35"/>
-      <c r="R37" s="39" t="s">
+      <c r="Q37" s="42"/>
+      <c r="R37" s="41" t="s">
         <v>115</v>
       </c>
-      <c r="S37" s="39"/>
+      <c r="S37" s="41"/>
       <c r="AC37" t="s">
         <v>54</v>
       </c>
@@ -2613,7 +2627,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="38" spans="3:30">
       <c r="C38" s="2">
         <v>14</v>
       </c>
@@ -2642,7 +2656,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="39" spans="3:30">
       <c r="C39" s="2">
         <v>15</v>
       </c>
@@ -2664,6 +2678,9 @@
         <f t="shared" ref="I39:I49" si="7">LOOKUP(H39,$C$4:$AA$4,$C$5:$AA$5)</f>
         <v>C2-6</v>
       </c>
+      <c r="N39" t="s">
+        <v>133</v>
+      </c>
       <c r="AC39" t="s">
         <v>55</v>
       </c>
@@ -2671,7 +2688,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="40" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="40" spans="3:30">
       <c r="C40" s="2">
         <v>16</v>
       </c>
@@ -2693,6 +2710,54 @@
         <f t="shared" si="7"/>
         <v>GND</v>
       </c>
+      <c r="L40" s="38" t="s">
+        <v>36</v>
+      </c>
+      <c r="M40" s="38" t="s">
+        <v>32</v>
+      </c>
+      <c r="N40" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="O40" s="38" t="s">
+        <v>31</v>
+      </c>
+      <c r="P40" s="38" t="s">
+        <v>34</v>
+      </c>
+      <c r="Q40" s="38" t="s">
+        <v>30</v>
+      </c>
+      <c r="R40" s="38" t="s">
+        <v>33</v>
+      </c>
+      <c r="S40" s="38" t="s">
+        <v>29</v>
+      </c>
+      <c r="T40" s="45" t="s">
+        <v>20</v>
+      </c>
+      <c r="U40" s="45" t="s">
+        <v>19</v>
+      </c>
+      <c r="V40" s="45" t="s">
+        <v>18</v>
+      </c>
+      <c r="W40" s="45" t="s">
+        <v>17</v>
+      </c>
+      <c r="X40" s="45" t="s">
+        <v>16</v>
+      </c>
+      <c r="Y40" s="45" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z40" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="AA40" s="45" t="s">
+        <v>13</v>
+      </c>
       <c r="AC40" t="s">
         <v>68</v>
       </c>
@@ -2700,7 +2765,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="41" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="41" spans="3:30">
       <c r="C41" s="2">
         <v>17</v>
       </c>
@@ -2722,6 +2787,54 @@
         <f t="shared" si="7"/>
         <v>C3-0</v>
       </c>
+      <c r="L41" s="34" t="s">
+        <v>123</v>
+      </c>
+      <c r="M41" s="34" t="s">
+        <v>105</v>
+      </c>
+      <c r="N41" s="34" t="s">
+        <v>124</v>
+      </c>
+      <c r="O41" s="34" t="s">
+        <v>106</v>
+      </c>
+      <c r="P41" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q41" s="34" t="s">
+        <v>103</v>
+      </c>
+      <c r="R41" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="S41" s="34" t="s">
+        <v>104</v>
+      </c>
+      <c r="T41" s="34" t="s">
+        <v>120</v>
+      </c>
+      <c r="U41" s="34" t="s">
+        <v>101</v>
+      </c>
+      <c r="V41" s="34" t="s">
+        <v>119</v>
+      </c>
+      <c r="W41" s="34" t="s">
+        <v>102</v>
+      </c>
+      <c r="X41" s="34" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y41" s="34" t="s">
+        <v>99</v>
+      </c>
+      <c r="Z41" s="34" t="s">
+        <v>117</v>
+      </c>
+      <c r="AA41" s="34" t="s">
+        <v>100</v>
+      </c>
       <c r="AC41" t="s">
         <v>56</v>
       </c>
@@ -2729,7 +2842,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="42" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="42" spans="3:30">
       <c r="C42" s="2">
         <v>18</v>
       </c>
@@ -2758,7 +2871,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="43" spans="3:30">
       <c r="C43" s="2">
         <v>19</v>
       </c>
@@ -2780,6 +2893,9 @@
         <f t="shared" si="7"/>
         <v>C3-4</v>
       </c>
+      <c r="N43" t="s">
+        <v>134</v>
+      </c>
       <c r="AC43" t="s">
         <v>58</v>
       </c>
@@ -2787,7 +2903,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="44" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="44" spans="3:30">
       <c r="C44" s="2">
         <v>20</v>
       </c>
@@ -2809,6 +2925,54 @@
         <f t="shared" si="7"/>
         <v>C3-6</v>
       </c>
+      <c r="L44" s="36" t="s">
+        <v>28</v>
+      </c>
+      <c r="M44" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="N44" s="36" t="s">
+        <v>27</v>
+      </c>
+      <c r="O44" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="P44" s="36" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q44" s="36" t="s">
+        <v>23</v>
+      </c>
+      <c r="R44" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="S44" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="T44" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="U44" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="V44" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="W44" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="X44" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="Y44" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="Z44" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="AA44" s="10" t="s">
+        <v>5</v>
+      </c>
       <c r="AC44" t="s">
         <v>71</v>
       </c>
@@ -2816,7 +2980,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="45" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="45" spans="3:30">
       <c r="C45" s="2">
         <v>21</v>
       </c>
@@ -2838,6 +3002,54 @@
         <f t="shared" si="7"/>
         <v>GND</v>
       </c>
+      <c r="L45" t="s">
+        <v>113</v>
+      </c>
+      <c r="M45" t="s">
+        <v>125</v>
+      </c>
+      <c r="N45" t="s">
+        <v>114</v>
+      </c>
+      <c r="O45" t="s">
+        <v>126</v>
+      </c>
+      <c r="P45" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>132</v>
+      </c>
+      <c r="R45" t="s">
+        <v>112</v>
+      </c>
+      <c r="S45" t="s">
+        <v>131</v>
+      </c>
+      <c r="T45" t="s">
+        <v>109</v>
+      </c>
+      <c r="U45" t="s">
+        <v>130</v>
+      </c>
+      <c r="V45" t="s">
+        <v>110</v>
+      </c>
+      <c r="W45" t="s">
+        <v>129</v>
+      </c>
+      <c r="X45" t="s">
+        <v>107</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>108</v>
+      </c>
+      <c r="AA45" t="s">
+        <v>127</v>
+      </c>
       <c r="AC45" t="s">
         <v>59</v>
       </c>
@@ -2845,7 +3057,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="46" spans="3:30">
       <c r="C46" s="2">
         <v>22</v>
       </c>
@@ -2874,7 +3086,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="47" spans="3:30">
       <c r="C47" s="2">
         <v>23</v>
       </c>
@@ -2903,7 +3115,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="48" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="48" spans="3:30">
       <c r="C48" s="2">
         <v>24</v>
       </c>
@@ -2932,7 +3144,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="49" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:30">
       <c r="C49" s="2">
         <v>25</v>
       </c>
@@ -2961,7 +3173,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="50" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="50" spans="3:30">
       <c r="AC50" t="s">
         <v>74</v>
       </c>
@@ -2969,7 +3181,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="51" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="51" spans="3:30">
       <c r="AC51" t="s">
         <v>88</v>
       </c>
@@ -2977,7 +3189,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="52" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="52" spans="3:30">
       <c r="AC52" t="s">
         <v>76</v>
       </c>
@@ -2985,7 +3197,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="53" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="53" spans="3:30">
       <c r="C53" s="3">
         <v>1</v>
       </c>
@@ -3068,7 +3280,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="54" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="54" spans="3:30">
       <c r="C54" s="4" t="str">
         <f>"+5V"</f>
         <v>+5V</v>
@@ -3152,7 +3364,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="55" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="55" spans="3:30">
       <c r="C55" s="2" t="s">
         <v>0</v>
       </c>
@@ -3235,7 +3447,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="56" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="56" spans="3:30">
       <c r="C56" s="1">
         <v>26</v>
       </c>
@@ -3318,7 +3530,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="57" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="57" spans="3:30">
       <c r="AC57" t="s">
         <v>91</v>
       </c>
@@ -3326,7 +3538,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="58" spans="3:30">
       <c r="AC58" t="s">
         <v>79</v>
       </c>
@@ -3334,7 +3546,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="59" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="59" spans="3:30">
       <c r="C59" s="3">
         <v>1</v>
       </c>
@@ -3417,7 +3629,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="60" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="60" spans="3:30">
       <c r="C60" s="12" t="str">
         <f t="shared" ref="C60:Y61" si="8">LOOKUP(C54,$AD$23:$AD$72,$AC$23:$AC$72)</f>
         <v>25b</v>
@@ -3467,7 +3679,7 @@
         <v>1</v>
       </c>
       <c r="P60" s="12" t="str">
-        <f t="shared" ref="P60:R60" si="9">LOOKUP(P54,$AD$23:$AD$72,$AC$23:$AC$72)</f>
+        <f t="shared" ref="P60:Q60" si="9">LOOKUP(P54,$AD$23:$AD$72,$AC$23:$AC$72)</f>
         <v>23a</v>
       </c>
       <c r="Q60" s="12" t="str">
@@ -3517,7 +3729,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="61" spans="3:30">
       <c r="C61" s="12" t="str">
         <f t="shared" si="8"/>
         <v>21b</v>
@@ -3603,7 +3815,7 @@
         <v>15a</v>
       </c>
       <c r="Z61" s="12" t="str">
-        <f t="shared" ref="X61:Z61" si="11">LOOKUP(Z55,$AD$23:$AD$72,$AC$23:$AC$72)</f>
+        <f t="shared" ref="Z61" si="11">LOOKUP(Z55,$AD$23:$AD$72,$AC$23:$AC$72)</f>
         <v>8a</v>
       </c>
       <c r="AA61" s="12" t="str">
@@ -3617,7 +3829,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="62" spans="3:30">
       <c r="C62" s="1">
         <v>26</v>
       </c>
@@ -3700,7 +3912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="63" spans="3:30">
       <c r="AC63" t="s">
         <v>87</v>
       </c>
@@ -3708,7 +3920,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="3:30" x14ac:dyDescent="0.25">
+    <row r="64" spans="3:30">
       <c r="AC64" t="s">
         <v>92</v>
       </c>
@@ -3716,7 +3928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="29:30" x14ac:dyDescent="0.25">
+    <row r="65" spans="29:30">
       <c r="AC65" t="s">
         <v>65</v>
       </c>
@@ -3724,7 +3936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="29:30" x14ac:dyDescent="0.25">
+    <row r="66" spans="29:30">
       <c r="AC66" t="s">
         <v>70</v>
       </c>
@@ -3732,7 +3944,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="29:30" x14ac:dyDescent="0.25">
+    <row r="67" spans="29:30">
       <c r="AC67" t="s">
         <v>75</v>
       </c>
@@ -3740,7 +3952,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="29:30" x14ac:dyDescent="0.25">
+    <row r="68" spans="29:30">
       <c r="AC68" t="s">
         <v>80</v>
       </c>
@@ -3748,7 +3960,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="29:30" x14ac:dyDescent="0.25">
+    <row r="69" spans="29:30">
       <c r="AC69" t="s">
         <v>81</v>
       </c>
@@ -3756,7 +3968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="29:30" x14ac:dyDescent="0.25">
+    <row r="70" spans="29:30">
       <c r="AC70" t="s">
         <v>82</v>
       </c>
@@ -3764,7 +3976,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="29:30" x14ac:dyDescent="0.25">
+    <row r="71" spans="29:30">
       <c r="AC71" t="s">
         <v>93</v>
       </c>
@@ -3772,7 +3984,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="29:30" x14ac:dyDescent="0.25">
+    <row r="72" spans="29:30">
       <c r="AC72" t="s">
         <v>94</v>
       </c>
@@ -3785,13 +3997,13 @@
     <sortCondition ref="AD23:AD72"/>
   </sortState>
   <mergeCells count="7">
+    <mergeCell ref="D9:U9"/>
+    <mergeCell ref="F22:L22"/>
     <mergeCell ref="R37:S37"/>
     <mergeCell ref="P37:Q37"/>
     <mergeCell ref="T22:Z22"/>
     <mergeCell ref="O15:T15"/>
     <mergeCell ref="E15:J15"/>
-    <mergeCell ref="D9:U9"/>
-    <mergeCell ref="F22:L22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="47" orientation="landscape" r:id="rId1"/>
@@ -3800,24 +4012,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Whoops, forgot to save before commit
</commit_message>
<xml_diff>
--- a/docs/GRP_Proto_Pins.xlsx
+++ b/docs/GRP_Proto_Pins.xlsx
@@ -12,6 +12,7 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -672,19 +673,19 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -730,7 +731,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -750,7 +751,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -785,7 +786,7 @@
         <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="" val="0"/>
+              <a14:useLocalDpi xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
             </a:ext>
           </a:extLst>
         </a:blip>
@@ -805,7 +806,7 @@
         <a:noFill/>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns="" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:solidFill>
                 <a:srgbClr val="FFFFFF"/>
               </a:solidFill>
@@ -1109,8 +1110,8 @@
   </sheetPr>
   <dimension ref="C4:AF72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="T46" sqref="T46"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="P48" sqref="P48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1432,26 +1433,26 @@
       </c>
     </row>
     <row r="9" spans="3:27" ht="23.25">
-      <c r="D9" s="44" t="s">
+      <c r="D9" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="E9" s="44"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="44"/>
-      <c r="H9" s="44"/>
-      <c r="I9" s="44"/>
-      <c r="J9" s="44"/>
-      <c r="K9" s="44"/>
-      <c r="L9" s="44"/>
-      <c r="M9" s="44"/>
-      <c r="N9" s="44"/>
-      <c r="O9" s="44"/>
-      <c r="P9" s="44"/>
-      <c r="Q9" s="44"/>
-      <c r="R9" s="44"/>
-      <c r="S9" s="44"/>
-      <c r="T9" s="44"/>
-      <c r="U9" s="44"/>
+      <c r="E9" s="42"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="42"/>
+      <c r="H9" s="42"/>
+      <c r="I9" s="42"/>
+      <c r="J9" s="42"/>
+      <c r="K9" s="42"/>
+      <c r="L9" s="42"/>
+      <c r="M9" s="42"/>
+      <c r="N9" s="42"/>
+      <c r="O9" s="42"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="42"/>
+      <c r="R9" s="42"/>
+      <c r="S9" s="42"/>
+      <c r="T9" s="42"/>
+      <c r="U9" s="42"/>
     </row>
     <row r="10" spans="3:27" ht="23.25">
       <c r="D10" s="11"/>
@@ -1555,26 +1556,26 @@
     </row>
     <row r="15" spans="3:27" ht="15" customHeight="1">
       <c r="D15" s="10"/>
-      <c r="E15" s="42" t="s">
+      <c r="E15" s="45" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="42"/>
-      <c r="G15" s="42"/>
-      <c r="H15" s="42"/>
-      <c r="I15" s="42"/>
-      <c r="J15" s="42"/>
+      <c r="F15" s="45"/>
+      <c r="G15" s="45"/>
+      <c r="H15" s="45"/>
+      <c r="I15" s="45"/>
+      <c r="J15" s="45"/>
       <c r="K15" s="10"/>
       <c r="L15" s="10"/>
       <c r="M15" s="10"/>
       <c r="N15" s="10"/>
-      <c r="O15" s="42" t="s">
+      <c r="O15" s="45" t="s">
         <v>3</v>
       </c>
-      <c r="P15" s="42"/>
-      <c r="Q15" s="42"/>
-      <c r="R15" s="42"/>
-      <c r="S15" s="42"/>
-      <c r="T15" s="42"/>
+      <c r="P15" s="45"/>
+      <c r="Q15" s="45"/>
+      <c r="R15" s="45"/>
+      <c r="S15" s="45"/>
+      <c r="T15" s="45"/>
       <c r="U15" s="10"/>
     </row>
     <row r="16" spans="3:27">
@@ -2612,14 +2613,14 @@
         <f t="shared" si="5"/>
         <v>+5V</v>
       </c>
-      <c r="P37" s="42" t="s">
+      <c r="P37" s="45" t="s">
         <v>116</v>
       </c>
-      <c r="Q37" s="42"/>
-      <c r="R37" s="41" t="s">
+      <c r="Q37" s="45"/>
+      <c r="R37" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="S37" s="41"/>
+      <c r="S37" s="44"/>
       <c r="AC37" t="s">
         <v>54</v>
       </c>
@@ -2734,28 +2735,28 @@
       <c r="S40" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="T40" s="45" t="s">
+      <c r="T40" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="U40" s="45" t="s">
+      <c r="U40" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="V40" s="45" t="s">
+      <c r="V40" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="W40" s="45" t="s">
+      <c r="W40" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="X40" s="45" t="s">
+      <c r="X40" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="Y40" s="45" t="s">
+      <c r="Y40" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="Z40" s="45" t="s">
+      <c r="Z40" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="AA40" s="45" t="s">
+      <c r="AA40" s="41" t="s">
         <v>13</v>
       </c>
       <c r="AC40" t="s">

</xml_diff>